<commit_message>
All enumerated lists used in web forms should contain a single value, not a dictionary of value/labels. Removing the spreadsheet.value.column and data.value.column so we just have value.column for both. Improving the __str__ function in the ApiError class, to make debugging a little easier. Adding a "validate_all" flask command, to help us track down any issues with current workflows in production (use this in concert with sync_with_testing) Fixed logs of tests. removed fact_runner.py, a very early and crufty bit of code.
</commit_message>
<xml_diff>
--- a/tests/data/enum_options_with_search/sponsors.xlsx
+++ b/tests/data/enum_options_with_search/sponsors.xlsx
@@ -252,12 +252,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -323,25 +323,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C1030"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30:C30"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.0390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="9.03"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>